<commit_message>
Correct HDR & ITEM counters
</commit_message>
<xml_diff>
--- a/BillMacros/BillMacrosTemplate.xlsx
+++ b/BillMacros/BillMacrosTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kobus.burger\Google Drive\VS solutions\BillMacros\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kobus.burger\Google Drive\VS solutions\BillMacros\BillMacros\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -501,9 +501,6 @@
     <t>- Note that the cell will show #NAME? because Excel does not recognise these counters but this is expected</t>
   </si>
   <si>
-    <t>- H0No, H1No, H2No, H3No &amp; HItNo are counters that can be inserted in a billsheet formula. These counters will be replaced with the actual values during page formatting</t>
-  </si>
-  <si>
     <t>ITEM3</t>
   </si>
   <si>
@@ -514,6 +511,9 @@
   </si>
   <si>
     <t>NOTE &amp; N</t>
+  </si>
+  <si>
+    <t>- H0, H1, H2, H3 &amp; It are counters that can be inserted in a billsheet formula. These counters will be replaced with the actual values during page formatting</t>
   </si>
 </sst>
 </file>
@@ -521,13 +521,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="7">
-    <numFmt numFmtId="170" formatCode="_ &quot;R&quot;\ * #,##0.00_ ;_ &quot;R&quot;\ * \-#,##0.00_ ;_ &quot;R&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="171" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="#,##0.00;\-#,##0.00;&quot;&quot;"/>
-    <numFmt numFmtId="181" formatCode="0.000"/>
-    <numFmt numFmtId="182" formatCode="&quot;Section &quot;#0"/>
-    <numFmt numFmtId="186" formatCode="yyyy/mm"/>
-    <numFmt numFmtId="191" formatCode="&quot;R&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="_ &quot;R&quot;\ * #,##0.00_ ;_ &quot;R&quot;\ * \-#,##0.00_ ;_ &quot;R&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="#,##0.00;\-#,##0.00;&quot;&quot;"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="&quot;Section &quot;#0"/>
+    <numFmt numFmtId="169" formatCode="yyyy/mm"/>
+    <numFmt numFmtId="170" formatCode="&quot;R&quot;#,##0.00"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -823,10 +823,10 @@
   </borders>
   <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
@@ -853,7 +853,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="182" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -862,14 +862,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -893,7 +893,7 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -907,16 +907,16 @@
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="171" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -927,19 +927,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -986,20 +986,20 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="180" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="186" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="180" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -1017,7 +1017,7 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -1044,23 +1044,23 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="180" fontId="4" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="180" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="180" fontId="4" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="182" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1072,29 +1072,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="180" fontId="4" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="180" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="180" fontId="4" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="180" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="180" fontId="4" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1128,7 +1128,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="5" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1147,7 +1147,7 @@
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1157,7 +1157,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="191" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1172,11 +1172,11 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -1196,7 +1196,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7"/>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
@@ -1553,7 +1553,7 @@
   <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1818,7 +1818,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B16" s="27"/>
       <c r="C16" s="44" t="e">
@@ -2175,7 +2175,7 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
@@ -2200,7 +2200,7 @@
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="115" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
@@ -2210,7 +2210,7 @@
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
@@ -2255,7 +2255,7 @@
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="116" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Removed short notations e.g. H0 & H1
</commit_message>
<xml_diff>
--- a/BillMacros/BillMacrosTemplate.xlsx
+++ b/BillMacros/BillMacrosTemplate.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="276" windowWidth="9396" windowHeight="6852" tabRatio="737"/>
+    <workbookView xWindow="120" yWindow="276" windowWidth="9396" windowHeight="6852" tabRatio="737" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="BillTemplate" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="157">
   <si>
     <t>Reference</t>
   </si>
@@ -504,16 +504,13 @@
     <t>ITEM3</t>
   </si>
   <si>
-    <t>IHDR, H0, IHDR1, H1, IHDR2, H2, IHDR3 &amp; H3</t>
-  </si>
-  <si>
-    <t>ITEM, I0, ITEM1, I1, ITEM2, I2, ITEM3 &amp; I3</t>
-  </si>
-  <si>
-    <t>NOTE &amp; N</t>
-  </si>
-  <si>
-    <t>- H0, H1, H2, H3 &amp; It are counters that can be inserted in a billsheet formula. These counters will be replaced with the actual values during page formatting</t>
+    <t>- H0No, H1No, H2No, H3No &amp; HItNo are counters that can be inserted in a billsheet formula. These counters will be replaced with the actual values during page formatting</t>
+  </si>
+  <si>
+    <t>ITEM, ITEM1, ITEM2, ITEM3</t>
+  </si>
+  <si>
+    <t>IHDR, IHDR1, IHDR2, IHDR3</t>
   </si>
 </sst>
 </file>
@@ -1552,8 +1549,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2175,7 +2172,7 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
@@ -2210,7 +2207,7 @@
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>156</v>
+        <v>118</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
@@ -2255,7 +2252,7 @@
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="116" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
@@ -2827,7 +2824,7 @@
   </sheetPr>
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add checks for errors in cells
</commit_message>
<xml_diff>
--- a/BillMacros/BillMacrosTemplate.xlsx
+++ b/BillMacros/BillMacrosTemplate.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kobus.burger\Google Drive\VS solutions\BillMacros\BillMacros\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A431B9-17BD-49C2-8E94-D662A7B6E6C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="276" windowWidth="9396" windowHeight="6852" tabRatio="737" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="276" windowWidth="9396" windowHeight="6852" tabRatio="737" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BillTemplate" sheetId="1" r:id="rId1"/>
@@ -35,7 +36,14 @@
     <definedName name="_xlnm.Print_Area" localSheetId="3">Summary!$B$1:$D$18</definedName>
     <definedName name="SumBillRow" localSheetId="1">SumTemplate!$A$3:$E$3</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -516,7 +524,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
     <numFmt numFmtId="164" formatCode="_ &quot;R&quot;\ * #,##0.00_ ;_ &quot;R&quot;\ * \-#,##0.00_ ;_ &quot;R&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
@@ -524,7 +532,7 @@
     <numFmt numFmtId="167" formatCode="0.000"/>
     <numFmt numFmtId="168" formatCode="&quot;Section &quot;#0"/>
     <numFmt numFmtId="169" formatCode="yyyy/mm"/>
-    <numFmt numFmtId="170" formatCode="&quot;R&quot;#,##0.00"/>
+    <numFmt numFmtId="172" formatCode="&quot;R&quot;#,##0;;"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -830,7 +838,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1132,14 +1140,10 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="20" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="4" fontId="5" fillId="0" borderId="2" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
@@ -1148,15 +1152,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
@@ -1199,18 +1194,32 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="172" fontId="5" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="172" fontId="5" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="5" fillId="0" borderId="2" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="172" fontId="5" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="172" fontId="5" fillId="0" borderId="20" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma 5" xfId="2"/>
-    <cellStyle name="Comma0" xfId="3"/>
+    <cellStyle name="Comma 5" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Comma0" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Currency" xfId="4" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="5"/>
-    <cellStyle name="Normal 3" xfId="6"/>
-    <cellStyle name="Normal 4" xfId="7"/>
-    <cellStyle name="Normal 6" xfId="8"/>
-    <cellStyle name="Normal_Bill of quantities" xfId="9"/>
+    <cellStyle name="Normal 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 4" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 6" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal_Bill of quantities" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1545,12 +1554,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1575,10 +1584,10 @@
       <c r="G1" s="45"/>
       <c r="H1" s="45"/>
       <c r="I1" s="16"/>
-      <c r="J1" s="102" t="s">
+      <c r="J1" s="100" t="s">
         <v>104</v>
       </c>
-      <c r="K1" s="119">
+      <c r="K1" s="114">
         <f>SUBTOTAL(9,K4:K65031)</f>
         <v>0</v>
       </c>
@@ -1711,7 +1720,7 @@
       </c>
       <c r="B10" s="27"/>
       <c r="C10" s="44" t="e">
-        <f>$I$1&amp;"-"&amp;h0no&amp;"-"&amp;h3no</f>
+        <f>$I$1&amp;"."&amp;h0no&amp;"."&amp;h3no</f>
         <v>#NAME?</v>
       </c>
       <c r="D10" s="28"/>
@@ -1730,15 +1739,15 @@
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="56"/>
-      <c r="C11" s="112"/>
+      <c r="C11" s="107"/>
       <c r="D11" s="28"/>
-      <c r="E11" s="108"/>
-      <c r="F11" s="109"/>
-      <c r="G11" s="110"/>
-      <c r="H11" s="110"/>
+      <c r="E11" s="103"/>
+      <c r="F11" s="104"/>
+      <c r="G11" s="105"/>
+      <c r="H11" s="105"/>
       <c r="I11" s="48"/>
-      <c r="J11" s="111"/>
-      <c r="K11" s="110"/>
+      <c r="J11" s="106"/>
+      <c r="K11" s="105"/>
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1747,7 +1756,7 @@
       </c>
       <c r="B12" s="27"/>
       <c r="C12" s="44" t="e">
-        <f>$I$1&amp;"-"&amp;h0no&amp;"-"&amp;h1no&amp;"-"&amp;h3no</f>
+        <f>$I$1&amp;"."&amp;h0no&amp;"."&amp;h1no&amp;"."&amp;h3no</f>
         <v>#NAME?</v>
       </c>
       <c r="D12" s="28"/>
@@ -1766,15 +1775,15 @@
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="56"/>
-      <c r="C13" s="112"/>
+      <c r="C13" s="107"/>
       <c r="D13" s="28"/>
-      <c r="E13" s="108"/>
-      <c r="F13" s="109"/>
-      <c r="G13" s="110"/>
-      <c r="H13" s="110"/>
+      <c r="E13" s="103"/>
+      <c r="F13" s="104"/>
+      <c r="G13" s="105"/>
+      <c r="H13" s="105"/>
       <c r="I13" s="48"/>
-      <c r="J13" s="111"/>
-      <c r="K13" s="110"/>
+      <c r="J13" s="106"/>
+      <c r="K13" s="105"/>
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1783,7 +1792,7 @@
       </c>
       <c r="B14" s="27"/>
       <c r="C14" s="44" t="e">
-        <f>$I$1&amp;"-"&amp;h0no&amp;"-"&amp;h1no&amp;"-"&amp;h2no&amp;"-"&amp;hitno</f>
+        <f>$I$1&amp;"."&amp;h0no&amp;"."&amp;h1no&amp;"."&amp;h2no&amp;"."&amp;hitno</f>
         <v>#NAME?</v>
       </c>
       <c r="D14" s="28"/>
@@ -1802,15 +1811,15 @@
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
       <c r="B15" s="56"/>
-      <c r="C15" s="112"/>
+      <c r="C15" s="107"/>
       <c r="D15" s="28"/>
-      <c r="E15" s="108"/>
-      <c r="F15" s="109"/>
-      <c r="G15" s="110"/>
-      <c r="H15" s="110"/>
+      <c r="E15" s="103"/>
+      <c r="F15" s="104"/>
+      <c r="G15" s="105"/>
+      <c r="H15" s="105"/>
       <c r="I15" s="48"/>
-      <c r="J15" s="111"/>
-      <c r="K15" s="110"/>
+      <c r="J15" s="106"/>
+      <c r="K15" s="105"/>
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1819,7 +1828,7 @@
       </c>
       <c r="B16" s="27"/>
       <c r="C16" s="44" t="e">
-        <f>$I$1&amp;"-"&amp;h0no&amp;"-"&amp;h1no&amp;"-"&amp;h2no&amp;"-"&amp;h3no&amp;"-"&amp;hitno</f>
+        <f>$I$1&amp;"."&amp;h0no&amp;"."&amp;h1no&amp;"."&amp;h2no&amp;"."&amp;h3no&amp;"."&amp;hitno</f>
         <v>#NAME?</v>
       </c>
       <c r="D16" s="28"/>
@@ -1853,7 +1862,7 @@
       </c>
       <c r="B18" s="27"/>
       <c r="C18" s="44" t="e">
-        <f>$I$1&amp;"-"&amp;h0no</f>
+        <f>$I$1&amp;"."&amp;h0no</f>
         <v>#NAME?</v>
       </c>
       <c r="D18" s="42"/>
@@ -1872,15 +1881,15 @@
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="56"/>
-      <c r="C19" s="107"/>
+      <c r="C19" s="102"/>
       <c r="D19" s="42"/>
-      <c r="E19" s="108"/>
-      <c r="F19" s="109"/>
-      <c r="G19" s="110"/>
-      <c r="H19" s="110"/>
+      <c r="E19" s="103"/>
+      <c r="F19" s="104"/>
+      <c r="G19" s="105"/>
+      <c r="H19" s="105"/>
       <c r="I19" s="48"/>
-      <c r="J19" s="111"/>
-      <c r="K19" s="110"/>
+      <c r="J19" s="106"/>
+      <c r="K19" s="105"/>
       <c r="L19" s="1"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1889,7 +1898,7 @@
       </c>
       <c r="B20" s="27"/>
       <c r="C20" s="44" t="e">
-        <f>$I$1&amp;"-"&amp;h0no&amp;"-"&amp;h1no</f>
+        <f>$I$1&amp;"."&amp;h0no&amp;"."&amp;h1no</f>
         <v>#NAME?</v>
       </c>
       <c r="D20" s="28"/>
@@ -1908,15 +1917,15 @@
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="56"/>
-      <c r="C21" s="107"/>
+      <c r="C21" s="102"/>
       <c r="D21" s="42"/>
-      <c r="E21" s="108"/>
-      <c r="F21" s="109"/>
-      <c r="G21" s="110"/>
-      <c r="H21" s="110"/>
+      <c r="E21" s="103"/>
+      <c r="F21" s="104"/>
+      <c r="G21" s="105"/>
+      <c r="H21" s="105"/>
       <c r="I21" s="48"/>
-      <c r="J21" s="111"/>
-      <c r="K21" s="110"/>
+      <c r="J21" s="106"/>
+      <c r="K21" s="105"/>
       <c r="L21" s="1"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -1925,7 +1934,7 @@
       </c>
       <c r="B22" s="27"/>
       <c r="C22" s="44" t="e">
-        <f>$I$1&amp;"-"&amp;h0no&amp;"-"&amp;h1no&amp;"-"&amp;h2no</f>
+        <f>$I$1&amp;"."&amp;h0no&amp;"."&amp;h1no&amp;"."&amp;h2no</f>
         <v>#NAME?</v>
       </c>
       <c r="D22" s="28"/>
@@ -1944,15 +1953,15 @@
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="17"/>
       <c r="B23" s="56"/>
-      <c r="C23" s="112"/>
+      <c r="C23" s="107"/>
       <c r="D23" s="28"/>
-      <c r="E23" s="108"/>
-      <c r="F23" s="109"/>
-      <c r="G23" s="110"/>
-      <c r="H23" s="110"/>
+      <c r="E23" s="103"/>
+      <c r="F23" s="104"/>
+      <c r="G23" s="105"/>
+      <c r="H23" s="105"/>
       <c r="I23" s="48"/>
-      <c r="J23" s="111"/>
-      <c r="K23" s="110"/>
+      <c r="J23" s="106"/>
+      <c r="K23" s="105"/>
       <c r="L23" s="1"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -1961,7 +1970,7 @@
       </c>
       <c r="B24" s="27"/>
       <c r="C24" s="44" t="e">
-        <f>$I$1&amp;"-"&amp;h0no&amp;"-"&amp;h1no&amp;"-"&amp;h2no</f>
+        <f>$I$1&amp;"."&amp;h0no&amp;"."&amp;h1no&amp;"."&amp;h2no</f>
         <v>#NAME?</v>
       </c>
       <c r="D24" s="28"/>
@@ -1980,15 +1989,15 @@
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="17"/>
       <c r="B25" s="56"/>
-      <c r="C25" s="112"/>
+      <c r="C25" s="107"/>
       <c r="D25" s="28"/>
-      <c r="E25" s="108"/>
-      <c r="F25" s="109"/>
-      <c r="G25" s="110"/>
-      <c r="H25" s="110"/>
+      <c r="E25" s="103"/>
+      <c r="F25" s="104"/>
+      <c r="G25" s="105"/>
+      <c r="H25" s="105"/>
       <c r="I25" s="48"/>
-      <c r="J25" s="111"/>
-      <c r="K25" s="110"/>
+      <c r="J25" s="106"/>
+      <c r="K25" s="105"/>
       <c r="L25" s="1"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -2020,11 +2029,11 @@
       <c r="G28" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="H28" s="101" t="s">
+      <c r="H28" s="99" t="s">
         <v>8</v>
       </c>
       <c r="I28" s="16"/>
-      <c r="K28" s="117">
+      <c r="K28" s="112">
         <f>SUBTOTAL(9,K$5:K27)</f>
         <v>0</v>
       </c>
@@ -2042,7 +2051,7 @@
       <c r="G29" s="59"/>
       <c r="H29" s="63"/>
       <c r="I29" s="16"/>
-      <c r="K29" s="118"/>
+      <c r="K29" s="113"/>
       <c r="L29" s="16"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -2057,7 +2066,7 @@
       <c r="G30" s="59"/>
       <c r="H30" s="62"/>
       <c r="I30" s="16"/>
-      <c r="K30" s="118"/>
+      <c r="K30" s="113"/>
       <c r="L30" s="16"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -2072,11 +2081,11 @@
       <c r="G31" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="H31" s="101" t="s">
+      <c r="H31" s="99" t="s">
         <v>8</v>
       </c>
       <c r="I31" s="16"/>
-      <c r="K31" s="117">
+      <c r="K31" s="112">
         <f>SUBTOTAL(9,K$5:K27)</f>
         <v>0</v>
       </c>
@@ -2126,7 +2135,7 @@
         <v>8</v>
       </c>
       <c r="I36" s="1"/>
-      <c r="K36" s="117">
+      <c r="K36" s="112">
         <f>SUBTOTAL(9,K$5:K35)</f>
         <v>0</v>
       </c>
@@ -2161,7 +2170,7 @@
       <c r="K39" s="29"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="103" t="s">
+      <c r="A42" s="101" t="s">
         <v>100</v>
       </c>
     </row>
@@ -2176,32 +2185,32 @@
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="115" t="s">
+      <c r="A45" s="110" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="115" t="s">
+      <c r="A46" s="110" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="115" t="s">
+      <c r="A47" s="110" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="116" t="s">
+      <c r="A48" s="111" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="115" t="s">
+      <c r="A49" s="110" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="115" t="s">
+      <c r="A50" s="110" t="s">
         <v>143</v>
       </c>
     </row>
@@ -2211,17 +2220,17 @@
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="116" t="s">
+      <c r="A52" s="111" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="116" t="s">
+      <c r="A53" s="111" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="116" t="s">
+      <c r="A54" s="111" t="s">
         <v>146</v>
       </c>
     </row>
@@ -2246,24 +2255,24 @@
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="116" t="s">
+      <c r="A59" s="111" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="116" t="s">
+      <c r="A60" s="111" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="116" t="s">
+      <c r="A61" s="111" t="s">
         <v>152</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E9 E17 E26:E34">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E9 E17 E26:E34" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"-,No,m,m²,m³,%,Prov Sum,Lump Sum,Sum, Litre, hour, day"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2274,12 +2283,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2294,24 +2303,26 @@
       </c>
       <c r="B1" s="46"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C3" s="105" t="str">
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="121"/>
+      <c r="B3" s="121"/>
+      <c r="C3" s="122" t="str">
         <f>BillTemplate!$B$1&amp;" "&amp;BillTemplate!$C$1</f>
         <v>Bill A: Test</v>
       </c>
-      <c r="D3" s="104" t="s">
+      <c r="D3" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="106">
+      <c r="E3" s="123">
         <f>BillTemplate!$K$1</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="103" t="s">
+      <c r="A7" s="101" t="s">
         <v>100</v>
       </c>
-      <c r="B7" s="103"/>
+      <c r="B7" s="101"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="46" t="s">
@@ -2356,7 +2367,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:C69"/>
   <sheetViews>
@@ -2517,7 +2528,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="103" t="s">
+      <c r="A24" s="101" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2722,7 +2733,7 @@
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="103" t="s">
+      <c r="A52" s="101" t="s">
         <v>100</v>
       </c>
     </row>
@@ -2747,62 +2758,62 @@
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="114" t="s">
+      <c r="A57" s="109" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="113" t="s">
+      <c r="A58" s="108" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="113" t="s">
+      <c r="A59" s="108" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="113" t="s">
+      <c r="A60" s="108" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="113" t="s">
+      <c r="A61" s="108" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="113" t="s">
+      <c r="A62" s="108" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="113" t="s">
+      <c r="A63" s="108" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="113" t="s">
+      <c r="A64" s="108" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="113" t="s">
+      <c r="A65" s="108" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="113" t="s">
+      <c r="A66" s="108" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="113" t="s">
+      <c r="A67" s="108" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="113" t="s">
+      <c r="A68" s="108" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2818,14 +2829,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet3">
     <tabColor rgb="FF00FF00"/>
   </sheetPr>
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2845,14 +2856,14 @@
         <v>16</v>
       </c>
       <c r="C1" s="90"/>
-      <c r="D1" s="96"/>
+      <c r="D1" s="95"/>
       <c r="E1" s="91"/>
     </row>
     <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="89"/>
       <c r="B2" s="89"/>
       <c r="C2" s="89"/>
-      <c r="D2" s="97"/>
+      <c r="D2" s="96"/>
       <c r="E2" s="91"/>
     </row>
     <row r="3" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.25">
@@ -2861,21 +2872,21 @@
         <v>17</v>
       </c>
       <c r="C3" s="90"/>
-      <c r="D3" s="97"/>
+      <c r="D3" s="96"/>
       <c r="E3" s="91"/>
     </row>
     <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="89"/>
       <c r="B4" s="89"/>
       <c r="C4" s="89"/>
-      <c r="D4" s="97"/>
+      <c r="D4" s="96"/>
       <c r="E4" s="91"/>
     </row>
     <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="89"/>
       <c r="B5" s="89"/>
       <c r="C5" s="89"/>
-      <c r="D5" s="97"/>
+      <c r="D5" s="96"/>
       <c r="E5" s="91"/>
     </row>
     <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -2884,7 +2895,7 @@
       </c>
       <c r="B6" s="89"/>
       <c r="C6" s="89"/>
-      <c r="D6" s="97"/>
+      <c r="D6" s="96"/>
       <c r="E6" s="91"/>
     </row>
     <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -2893,14 +2904,14 @@
       </c>
       <c r="B7" s="89"/>
       <c r="C7" s="89"/>
-      <c r="D7" s="98"/>
+      <c r="D7" s="97"/>
       <c r="E7" s="92"/>
     </row>
     <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="89"/>
       <c r="B8" s="89"/>
       <c r="C8" s="89"/>
-      <c r="D8" s="99"/>
+      <c r="D8" s="98"/>
       <c r="E8" s="92"/>
     </row>
     <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -2909,31 +2920,31 @@
         <v>20</v>
       </c>
       <c r="C9" s="89"/>
-      <c r="D9" s="99" t="s">
+      <c r="D9" s="116" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="92">
+      <c r="E9" s="117">
         <f>SUM(E6:E7)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="89"/>
-      <c r="B10" s="97"/>
+      <c r="B10" s="96"/>
       <c r="C10" s="89"/>
-      <c r="D10" s="99"/>
-      <c r="E10" s="92"/>
+      <c r="D10" s="116"/>
+      <c r="E10" s="117"/>
     </row>
     <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="89"/>
-      <c r="B11" s="97" t="s">
+      <c r="B11" s="96" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="93"/>
-      <c r="D11" s="99" t="s">
+      <c r="D11" s="116" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="92">
+      <c r="E11" s="117">
         <f>10%*E9</f>
         <v>0</v>
       </c>
@@ -2942,15 +2953,15 @@
       <c r="A12" s="89"/>
       <c r="B12" s="93"/>
       <c r="C12" s="93"/>
-      <c r="D12" s="98"/>
-      <c r="E12" s="92"/>
+      <c r="D12" s="118"/>
+      <c r="E12" s="117"/>
     </row>
     <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="89"/>
       <c r="B13" s="89"/>
       <c r="C13" s="89"/>
-      <c r="D13" s="99"/>
-      <c r="E13" s="92"/>
+      <c r="D13" s="116"/>
+      <c r="E13" s="117"/>
     </row>
     <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="89"/>
@@ -2958,10 +2969,10 @@
         <v>22</v>
       </c>
       <c r="C14" s="89"/>
-      <c r="D14" s="99" t="s">
+      <c r="D14" s="116" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="92">
+      <c r="E14" s="117">
         <f>SUM(E8:E13)</f>
         <v>0</v>
       </c>
@@ -2970,8 +2981,8 @@
       <c r="A15" s="89"/>
       <c r="B15" s="89"/>
       <c r="C15" s="89"/>
-      <c r="D15" s="99"/>
-      <c r="E15" s="92"/>
+      <c r="D15" s="116"/>
+      <c r="E15" s="117"/>
     </row>
     <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="89"/>
@@ -2979,10 +2990,10 @@
         <v>23</v>
       </c>
       <c r="C16" s="89"/>
-      <c r="D16" s="100" t="s">
+      <c r="D16" s="119" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="92">
+      <c r="E16" s="117">
         <f>14%*E14</f>
         <v>0</v>
       </c>
@@ -2991,21 +3002,21 @@
       <c r="A17" s="89"/>
       <c r="B17" s="89"/>
       <c r="C17" s="89"/>
-      <c r="D17" s="100"/>
-      <c r="E17" s="92"/>
+      <c r="D17" s="119"/>
+      <c r="E17" s="117"/>
     </row>
     <row r="18" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="93" t="s">
         <v>96</v>
       </c>
-      <c r="B18" s="120" t="s">
+      <c r="B18" s="115" t="s">
         <v>24</v>
       </c>
       <c r="C18" s="94"/>
-      <c r="D18" s="95" t="s">
+      <c r="D18" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="92">
+      <c r="E18" s="117">
         <f>SUM(E13:E17)</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
corrected ReplaceFormulaRefs loop in CheckTemplateSheet
</commit_message>
<xml_diff>
--- a/BillMacros/BillMacrosTemplate.xlsx
+++ b/BillMacros/BillMacrosTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kobus.burger\Google Drive\VS solutions\BillMacros\BillMacros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A431B9-17BD-49C2-8E94-D662A7B6E6C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B407637D-B1C1-4192-8421-B75AD84E385C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="276" windowWidth="9396" windowHeight="6852" tabRatio="737" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="270" windowWidth="9390" windowHeight="6855" tabRatio="737" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BillTemplate" sheetId="1" r:id="rId1"/>
@@ -362,18 +362,12 @@
     <t>Insert "returns" (Alt-Enter) in column A to make the row higher</t>
   </si>
   <si>
-    <t>Estimate</t>
-  </si>
-  <si>
     <t>Test</t>
   </si>
   <si>
     <t>Bill A:</t>
   </si>
   <si>
-    <t>Use absolute references in the formules</t>
-  </si>
-  <si>
     <t>This sheet contains info that is used to set up the page layout</t>
   </si>
   <si>
@@ -519,6 +513,12 @@
   </si>
   <si>
     <t>IHDR, IHDR1, IHDR2, IHDR3</t>
+  </si>
+  <si>
+    <t>NB: Use absolute references in the formules and ensure that it preceded by a sheet name</t>
+  </si>
+  <si>
+    <t>Only formats are copied to billsheet, not content</t>
   </si>
 </sst>
 </file>
@@ -532,7 +532,7 @@
     <numFmt numFmtId="167" formatCode="0.000"/>
     <numFmt numFmtId="168" formatCode="&quot;Section &quot;#0"/>
     <numFmt numFmtId="169" formatCode="yyyy/mm"/>
-    <numFmt numFmtId="172" formatCode="&quot;R&quot;#,##0;;"/>
+    <numFmt numFmtId="170" formatCode="&quot;R&quot;#,##0;;"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -1194,18 +1194,18 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="5" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="172" fontId="5" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="5" fillId="0" borderId="2" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="172" fontId="5" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="172" fontId="5" fillId="0" borderId="20" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="5" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="170" fontId="5" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="5" fillId="0" borderId="2" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="170" fontId="5" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="170" fontId="5" fillId="0" borderId="20" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1556,27 +1556,27 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L61"/>
+  <dimension ref="A1:M61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.88671875" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>97</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
@@ -1584,15 +1584,13 @@
       <c r="G1" s="45"/>
       <c r="H1" s="45"/>
       <c r="I1" s="16"/>
-      <c r="J1" s="100" t="s">
-        <v>104</v>
-      </c>
-      <c r="K1" s="114">
-        <f>SUBTOTAL(9,K4:K65031)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J1" s="100"/>
+      <c r="K1" s="114"/>
+      <c r="M1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
       <c r="C2" s="8"/>
@@ -1606,7 +1604,7 @@
       <c r="K2" s="23"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>13</v>
       </c>
@@ -1622,7 +1620,7 @@
       <c r="K3" s="79"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>13</v>
       </c>
@@ -1655,7 +1653,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>13</v>
       </c>
@@ -1670,7 +1668,7 @@
       <c r="J5" s="78"/>
       <c r="K5" s="80"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="17"/>
       <c r="B6" s="24"/>
       <c r="C6" s="24"/>
@@ -1683,12 +1681,12 @@
       <c r="J6" s="26"/>
       <c r="K6" s="25"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="F7" s="53"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="33"/>
@@ -1702,7 +1700,7 @@
       <c r="K8" s="35"/>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B9" s="40"/>
       <c r="C9" s="40"/>
       <c r="D9" s="40"/>
@@ -1714,9 +1712,9 @@
       <c r="J9" s="40"/>
       <c r="K9" s="40"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B10" s="27"/>
       <c r="C10" s="44" t="e">
@@ -1736,7 +1734,7 @@
       </c>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" s="56"/>
       <c r="C11" s="107"/>
@@ -1750,9 +1748,9 @@
       <c r="K11" s="105"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B12" s="27"/>
       <c r="C12" s="44" t="e">
@@ -1772,7 +1770,7 @@
       </c>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="B13" s="56"/>
       <c r="C13" s="107"/>
@@ -1786,9 +1784,9 @@
       <c r="K13" s="105"/>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B14" s="27"/>
       <c r="C14" s="44" t="e">
@@ -1808,7 +1806,7 @@
       </c>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="17"/>
       <c r="B15" s="56"/>
       <c r="C15" s="107"/>
@@ -1822,9 +1820,9 @@
       <c r="K15" s="105"/>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B16" s="27"/>
       <c r="C16" s="44" t="e">
@@ -1844,7 +1842,7 @@
       </c>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B17" s="40"/>
       <c r="C17" s="40"/>
       <c r="D17" s="40"/>
@@ -1856,7 +1854,7 @@
       <c r="J17" s="40"/>
       <c r="K17" s="40"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>14</v>
       </c>
@@ -1878,7 +1876,7 @@
       </c>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
       <c r="B19" s="56"/>
       <c r="C19" s="102"/>
@@ -1892,9 +1890,9 @@
       <c r="K19" s="105"/>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B20" s="27"/>
       <c r="C20" s="44" t="e">
@@ -1914,7 +1912,7 @@
       </c>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
       <c r="B21" s="56"/>
       <c r="C21" s="102"/>
@@ -1928,9 +1926,9 @@
       <c r="K21" s="105"/>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B22" s="27"/>
       <c r="C22" s="44" t="e">
@@ -1950,7 +1948,7 @@
       </c>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="17"/>
       <c r="B23" s="56"/>
       <c r="C23" s="107"/>
@@ -1964,9 +1962,9 @@
       <c r="K23" s="105"/>
       <c r="L23" s="1"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B24" s="27"/>
       <c r="C24" s="44" t="e">
@@ -1986,7 +1984,7 @@
       </c>
       <c r="L24" s="1"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="17"/>
       <c r="B25" s="56"/>
       <c r="C25" s="107"/>
@@ -2000,10 +1998,10 @@
       <c r="K25" s="105"/>
       <c r="L25" s="1"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F26" s="51"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
         <v>12</v>
       </c>
@@ -2017,7 +2015,7 @@
       <c r="I27" s="16"/>
       <c r="L27" s="16"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
         <v>12</v>
       </c>
@@ -2039,7 +2037,7 @@
       </c>
       <c r="L28" s="16"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
         <v>12</v>
       </c>
@@ -2054,7 +2052,7 @@
       <c r="K29" s="113"/>
       <c r="L29" s="16"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
         <v>12</v>
       </c>
@@ -2069,7 +2067,7 @@
       <c r="K30" s="113"/>
       <c r="L30" s="16"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
         <v>12</v>
       </c>
@@ -2091,7 +2089,7 @@
       </c>
       <c r="L31" s="16"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
         <v>12</v>
       </c>
@@ -2105,7 +2103,7 @@
       <c r="I32" s="16"/>
       <c r="L32" s="16"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>9</v>
       </c>
@@ -2119,7 +2117,7 @@
       <c r="I35" s="1"/>
       <c r="L35" s="1"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>9</v>
       </c>
@@ -2141,7 +2139,7 @@
       </c>
       <c r="L36" s="1"/>
     </row>
-    <row r="37" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>9</v>
       </c>
@@ -2155,8 +2153,8 @@
       <c r="I37" s="1"/>
       <c r="L37" s="1"/>
     </row>
-    <row r="38" spans="1:12" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="17"/>
       <c r="B39" s="27"/>
       <c r="C39" s="44"/>
@@ -2169,104 +2167,104 @@
       <c r="J39" s="32"/>
       <c r="K39" s="29"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="101" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A45" s="110" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A46" s="110" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A47" s="110" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A48" s="111" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="110" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="110" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" s="111" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" s="111" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" s="111" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="110" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="110" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="110" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="111" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="110" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="110" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" s="46" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" s="46" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="111" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="111" t="s">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" s="46" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" s="46" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" s="111" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="111" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="46" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="46" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="46" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="46" t="s">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" s="111" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" s="111" t="s">
         <v>150</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="111" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="111" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="111" t="s">
-        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -2288,22 +2286,22 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="42.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="42.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="46" t="s">
         <v>98</v>
       </c>
       <c r="B1" s="46"/>
     </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="121"/>
       <c r="B3" s="121"/>
       <c r="C3" s="122" t="str">
@@ -2318,43 +2316,43 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="101" t="s">
         <v>100</v>
       </c>
       <c r="B7" s="101"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="46" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B8" s="46"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="46" t="s">
         <v>101</v>
       </c>
       <c r="B9" s="46"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="46" t="s">
         <v>99</v>
       </c>
       <c r="B10" s="46"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="46" t="s">
-        <v>107</v>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="101" t="s">
+        <v>155</v>
       </c>
       <c r="B11" s="46"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="46" t="s">
         <v>102</v>
       </c>
       <c r="B12" s="46"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="46" t="s">
         <v>103</v>
       </c>
@@ -2375,21 +2373,21 @@
       <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.109375" customWidth="1"/>
-    <col min="2" max="2" width="16.77734375" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>25</v>
       </c>
       <c r="B1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -2397,7 +2395,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -2405,12 +2403,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -2418,7 +2416,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -2426,7 +2424,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -2434,7 +2432,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -2442,21 +2440,21 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="B13" t="s">
-        <v>110</v>
-      </c>
-      <c r="C13" s="46" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -2467,7 +2465,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -2478,7 +2476,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -2489,7 +2487,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -2500,7 +2498,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>40</v>
       </c>
@@ -2511,7 +2509,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>41</v>
       </c>
@@ -2522,17 +2520,17 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="101" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -2540,7 +2538,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -2548,7 +2546,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>47</v>
       </c>
@@ -2556,7 +2554,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>49</v>
       </c>
@@ -2564,7 +2562,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>51</v>
       </c>
@@ -2572,7 +2570,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -2580,7 +2578,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>55</v>
       </c>
@@ -2588,7 +2586,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>57</v>
       </c>
@@ -2596,7 +2594,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>59</v>
       </c>
@@ -2604,7 +2602,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>61</v>
       </c>
@@ -2612,7 +2610,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>63</v>
       </c>
@@ -2620,7 +2618,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>65</v>
       </c>
@@ -2628,7 +2626,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>67</v>
       </c>
@@ -2636,7 +2634,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>69</v>
       </c>
@@ -2644,7 +2642,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>71</v>
       </c>
@@ -2652,7 +2650,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>73</v>
       </c>
@@ -2660,7 +2658,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>75</v>
       </c>
@@ -2668,7 +2666,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>77</v>
       </c>
@@ -2676,7 +2674,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>79</v>
       </c>
@@ -2684,7 +2682,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>81</v>
       </c>
@@ -2692,7 +2690,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>83</v>
       </c>
@@ -2700,7 +2698,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>85</v>
       </c>
@@ -2708,7 +2706,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>87</v>
       </c>
@@ -2716,7 +2714,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>89</v>
       </c>
@@ -2724,7 +2722,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>91</v>
       </c>
@@ -2732,94 +2730,94 @@
         <v>92</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="101" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="46" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="109" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="108" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="108" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="108" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="108" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="108" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="108" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="108" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" s="108" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" s="108" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" s="108" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" s="108" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>125</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="46" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="109" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="108" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="108" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="108" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="108" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="108" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="108" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="108" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="108" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="108" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="108" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="108" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -2839,16 +2837,16 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" customWidth="1"/>
-    <col min="3" max="3" width="61.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" customWidth="1"/>
+    <col min="3" max="3" width="61.7109375" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="89" t="s">
         <v>15</v>
       </c>
@@ -2859,14 +2857,14 @@
       <c r="D1" s="95"/>
       <c r="E1" s="91"/>
     </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="89"/>
       <c r="B2" s="89"/>
       <c r="C2" s="89"/>
       <c r="D2" s="96"/>
       <c r="E2" s="91"/>
     </row>
-    <row r="3" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="89"/>
       <c r="B3" s="90" t="s">
         <v>17</v>
@@ -2875,21 +2873,21 @@
       <c r="D3" s="96"/>
       <c r="E3" s="91"/>
     </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="89"/>
       <c r="B4" s="89"/>
       <c r="C4" s="89"/>
       <c r="D4" s="96"/>
       <c r="E4" s="91"/>
     </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="89"/>
       <c r="B5" s="89"/>
       <c r="C5" s="89"/>
       <c r="D5" s="96"/>
       <c r="E5" s="91"/>
     </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="89" t="s">
         <v>18</v>
       </c>
@@ -2898,7 +2896,7 @@
       <c r="D6" s="96"/>
       <c r="E6" s="91"/>
     </row>
-    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="89" t="s">
         <v>19</v>
       </c>
@@ -2907,14 +2905,14 @@
       <c r="D7" s="97"/>
       <c r="E7" s="92"/>
     </row>
-    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="89"/>
       <c r="B8" s="89"/>
       <c r="C8" s="89"/>
       <c r="D8" s="98"/>
       <c r="E8" s="92"/>
     </row>
-    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="89"/>
       <c r="B9" s="89" t="s">
         <v>20</v>
@@ -2928,14 +2926,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="89"/>
       <c r="B10" s="96"/>
       <c r="C10" s="89"/>
       <c r="D10" s="116"/>
       <c r="E10" s="117"/>
     </row>
-    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="89"/>
       <c r="B11" s="96" t="s">
         <v>21</v>
@@ -2949,21 +2947,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="89"/>
       <c r="B12" s="93"/>
       <c r="C12" s="93"/>
       <c r="D12" s="118"/>
       <c r="E12" s="117"/>
     </row>
-    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="89"/>
       <c r="B13" s="89"/>
       <c r="C13" s="89"/>
       <c r="D13" s="116"/>
       <c r="E13" s="117"/>
     </row>
-    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="89"/>
       <c r="B14" s="89" t="s">
         <v>22</v>
@@ -2977,14 +2975,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="89"/>
       <c r="B15" s="89"/>
       <c r="C15" s="89"/>
       <c r="D15" s="116"/>
       <c r="E15" s="117"/>
     </row>
-    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="89"/>
       <c r="B16" s="89" t="s">
         <v>23</v>
@@ -2998,14 +2996,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="89"/>
       <c r="B17" s="89"/>
       <c r="C17" s="89"/>
       <c r="D17" s="119"/>
       <c r="E17" s="117"/>
     </row>
-    <row r="18" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="93" t="s">
         <v>96</v>
       </c>
@@ -3021,7 +3019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:5" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Add "columns" range to templates
</commit_message>
<xml_diff>
--- a/BillMacros/BillMacrosTemplate.xlsx
+++ b/BillMacros/BillMacrosTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kobus.burger\Google Drive\VS solutions\BillMacros\BillMacros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B407637D-B1C1-4192-8421-B75AD84E385C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47355F0A-9683-4647-8CA7-EC04E3B62D13}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="270" windowWidth="9390" windowHeight="6855" tabRatio="737" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8415" yWindow="-15660" windowWidth="18300" windowHeight="15075" tabRatio="737" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BillTemplate" sheetId="1" r:id="rId1"/>
@@ -19,28 +19,34 @@
     <sheet name="Summary" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="BillEnd" localSheetId="0">BillTemplate!$A$35:$K$37</definedName>
+    <definedName name="BillEnd" localSheetId="0">BillTemplate!$A$37:$K$39</definedName>
     <definedName name="BillSheet" localSheetId="0">BillTemplate!$A$1:$K$1</definedName>
-    <definedName name="Blank" localSheetId="0">BillTemplate!$A$39:$K$39</definedName>
-    <definedName name="ColHDR" localSheetId="0">BillTemplate!$A$3:$K$5</definedName>
-    <definedName name="IHDR" localSheetId="0">BillTemplate!$A$18:$K$18</definedName>
-    <definedName name="IHDR1" localSheetId="0">BillTemplate!$A$20:$K$20</definedName>
-    <definedName name="IHDR2" localSheetId="0">BillTemplate!$A$22:$K$22</definedName>
-    <definedName name="IHDR3" localSheetId="0">BillTemplate!$A$24:$K$24</definedName>
-    <definedName name="Item" localSheetId="0">BillTemplate!$A$10:$K$10</definedName>
-    <definedName name="ITEM1" localSheetId="0">BillTemplate!$A$12:$K$12</definedName>
-    <definedName name="ITEM2" localSheetId="0">BillTemplate!$A$14:$K$14</definedName>
-    <definedName name="ITEM3" localSheetId="0">BillTemplate!$A$16:$K$16</definedName>
-    <definedName name="Note" localSheetId="0">BillTemplate!$A$8:$K$8</definedName>
-    <definedName name="PB" localSheetId="0">BillTemplate!$A$27:$K$32</definedName>
+    <definedName name="Blank" localSheetId="0">BillTemplate!$A$41:$K$41</definedName>
+    <definedName name="ColHDR" localSheetId="0">BillTemplate!$A$5:$K$7</definedName>
+    <definedName name="Columns" localSheetId="0">BillTemplate!$A$3:$K$3</definedName>
+    <definedName name="Columns" localSheetId="1">SumTemplate!$A$3:$E$3</definedName>
+    <definedName name="IHDR" localSheetId="0">BillTemplate!$A$20:$K$20</definedName>
+    <definedName name="IHDR1" localSheetId="0">BillTemplate!$A$22:$K$22</definedName>
+    <definedName name="IHDR2" localSheetId="0">BillTemplate!$A$24:$K$24</definedName>
+    <definedName name="IHDR3" localSheetId="0">BillTemplate!$A$26:$K$26</definedName>
+    <definedName name="Item" localSheetId="0">BillTemplate!$A$12:$K$12</definedName>
+    <definedName name="ITEM1" localSheetId="0">BillTemplate!$A$14:$K$14</definedName>
+    <definedName name="ITEM2" localSheetId="0">BillTemplate!$A$16:$K$16</definedName>
+    <definedName name="ITEM3" localSheetId="0">BillTemplate!$A$18:$K$18</definedName>
+    <definedName name="Note" localSheetId="0">BillTemplate!$A$10:$K$10</definedName>
+    <definedName name="PB" localSheetId="0">BillTemplate!$A$29:$K$34</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">Summary!$B$1:$D$18</definedName>
-    <definedName name="SumBillRow" localSheetId="1">SumTemplate!$A$3:$E$3</definedName>
+    <definedName name="SumBillRow" localSheetId="1">SumTemplate!$A$5:$E$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -48,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="171">
   <si>
     <t>Reference</t>
   </si>
@@ -519,6 +525,48 @@
   </si>
   <si>
     <t>Only formats are copied to billsheet, not content</t>
+  </si>
+  <si>
+    <t>#RefCol</t>
+  </si>
+  <si>
+    <t>#ItemNoCol</t>
+  </si>
+  <si>
+    <t>#DescrCol</t>
+  </si>
+  <si>
+    <t>#UnitCol</t>
+  </si>
+  <si>
+    <t>#QtyCol</t>
+  </si>
+  <si>
+    <t>#RateCol</t>
+  </si>
+  <si>
+    <t>#AmtCol</t>
+  </si>
+  <si>
+    <t>#PricedRateCol</t>
+  </si>
+  <si>
+    <t>#PricedAmtCol</t>
+  </si>
+  <si>
+    <t>#SumNoCol</t>
+  </si>
+  <si>
+    <t>#SumDesrCol</t>
+  </si>
+  <si>
+    <t>#SumAmtCol</t>
+  </si>
+  <si>
+    <t>#SumPricedAmtCol</t>
+  </si>
+  <si>
+    <t>The "Columns" named range is used to identify the type of column and is used in the calculations</t>
   </si>
 </sst>
 </file>
@@ -534,7 +582,7 @@
     <numFmt numFmtId="169" formatCode="yyyy/mm"/>
     <numFmt numFmtId="170" formatCode="&quot;R&quot;#,##0;;"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -576,6 +624,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -838,7 +891,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1208,6 +1261,7 @@
     <xf numFmtId="170" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="7" applyFont="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1556,10 +1610,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M61"/>
+  <dimension ref="A1:M64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1590,171 +1644,179 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="16"/>
+      <c r="B2" s="8"/>
       <c r="C2" s="8"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="1"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="114"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="69"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="77"/>
-      <c r="K3" s="79"/>
-      <c r="L3" s="1"/>
-    </row>
-    <row r="4" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="64" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="65" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="65" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="66" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="67" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="68" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4" s="17"/>
-      <c r="J4" s="67" t="s">
-        <v>5</v>
-      </c>
-      <c r="K4" s="68" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
+      <c r="B3" s="124" t="s">
+        <v>157</v>
+      </c>
+      <c r="C3" s="124" t="s">
+        <v>158</v>
+      </c>
+      <c r="D3" s="124" t="s">
+        <v>159</v>
+      </c>
+      <c r="E3" s="124" t="s">
+        <v>160</v>
+      </c>
+      <c r="F3" s="124" t="s">
+        <v>161</v>
+      </c>
+      <c r="G3" s="124" t="s">
+        <v>162</v>
+      </c>
+      <c r="H3" s="124" t="s">
+        <v>163</v>
+      </c>
+      <c r="I3" s="124"/>
+      <c r="J3" s="124" t="s">
+        <v>164</v>
+      </c>
+      <c r="K3" s="124" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="74"/>
-      <c r="C5" s="75"/>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="76"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="80"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="80"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="17"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="25"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="F7" s="53"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="77"/>
+      <c r="K5" s="79"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="66" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="68" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="17"/>
+      <c r="J6" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="K6" s="68" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="74"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="78"/>
+      <c r="H7" s="80"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="78"/>
+      <c r="K7" s="80"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="52"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="48"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="1"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="25"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B9" s="40"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="40"/>
+      <c r="F9" s="53"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="44" t="e">
-        <f>$I$1&amp;"."&amp;h0no&amp;"."&amp;h3no</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D10" s="28"/>
-      <c r="E10" s="41"/>
+        <v>116</v>
+      </c>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="34"/>
       <c r="F10" s="52"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="31"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="37"/>
       <c r="I10" s="48"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="29">
-        <f>IF(ISNUMBER(F10),J10*F10,IF(ISNUMBER(H10),H10,J10))</f>
-        <v>0</v>
-      </c>
+      <c r="J10" s="38"/>
+      <c r="K10" s="35"/>
       <c r="L10" s="1"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="56"/>
-      <c r="C11" s="107"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="103"/>
-      <c r="F11" s="104"/>
-      <c r="G11" s="105"/>
-      <c r="H11" s="105"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="106"/>
-      <c r="K11" s="105"/>
-      <c r="L11" s="1"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
+      <c r="K11" s="40"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B12" s="27"/>
       <c r="C12" s="44" t="e">
-        <f>$I$1&amp;"."&amp;h0no&amp;"."&amp;h1no&amp;"."&amp;h3no</f>
+        <f>$I$1&amp;"."&amp;h0no&amp;"."&amp;h3no</f>
         <v>#NAME?</v>
       </c>
       <c r="D12" s="28"/>
@@ -1786,11 +1848,11 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B14" s="27"/>
       <c r="C14" s="44" t="e">
-        <f>$I$1&amp;"."&amp;h0no&amp;"."&amp;h1no&amp;"."&amp;h2no&amp;"."&amp;hitno</f>
+        <f>$I$1&amp;"."&amp;h0no&amp;"."&amp;h1no&amp;"."&amp;h3no</f>
         <v>#NAME?</v>
       </c>
       <c r="D14" s="28"/>
@@ -1807,7 +1869,7 @@
       <c r="L14" s="1"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="17"/>
+      <c r="A15" s="6"/>
       <c r="B15" s="56"/>
       <c r="C15" s="107"/>
       <c r="D15" s="28"/>
@@ -1822,11 +1884,11 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
-        <v>151</v>
+        <v>113</v>
       </c>
       <c r="B16" s="27"/>
       <c r="C16" s="44" t="e">
-        <f>$I$1&amp;"."&amp;h0no&amp;"."&amp;h1no&amp;"."&amp;h2no&amp;"."&amp;h3no&amp;"."&amp;hitno</f>
+        <f>$I$1&amp;"."&amp;h0no&amp;"."&amp;h1no&amp;"."&amp;h2no&amp;"."&amp;hitno</f>
         <v>#NAME?</v>
       </c>
       <c r="D16" s="28"/>
@@ -1843,27 +1905,29 @@
       <c r="L16" s="1"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B17" s="40"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
-      <c r="K17" s="40"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="56"/>
+      <c r="C17" s="107"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="103"/>
+      <c r="F17" s="104"/>
+      <c r="G17" s="105"/>
+      <c r="H17" s="105"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="106"/>
+      <c r="K17" s="105"/>
+      <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
-        <v>14</v>
+      <c r="A18" s="17" t="s">
+        <v>151</v>
       </c>
       <c r="B18" s="27"/>
       <c r="C18" s="44" t="e">
-        <f>$I$1&amp;"."&amp;h0no</f>
+        <f>$I$1&amp;"."&amp;h0no&amp;"."&amp;h1no&amp;"."&amp;h2no&amp;"."&amp;h3no&amp;"."&amp;hitno</f>
         <v>#NAME?</v>
       </c>
-      <c r="D18" s="42"/>
+      <c r="D18" s="28"/>
       <c r="E18" s="41"/>
       <c r="F18" s="52"/>
       <c r="G18" s="30"/>
@@ -1877,29 +1941,27 @@
       <c r="L18" s="1"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="6"/>
-      <c r="B19" s="56"/>
-      <c r="C19" s="102"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="103"/>
-      <c r="F19" s="104"/>
-      <c r="G19" s="105"/>
-      <c r="H19" s="105"/>
-      <c r="I19" s="48"/>
-      <c r="J19" s="106"/>
-      <c r="K19" s="105"/>
-      <c r="L19" s="1"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="40"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="17" t="s">
-        <v>110</v>
+      <c r="A20" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="B20" s="27"/>
       <c r="C20" s="44" t="e">
-        <f>$I$1&amp;"."&amp;h0no&amp;"."&amp;h1no</f>
+        <f>$I$1&amp;"."&amp;h0no</f>
         <v>#NAME?</v>
       </c>
-      <c r="D20" s="28"/>
+      <c r="D20" s="42"/>
       <c r="E20" s="41"/>
       <c r="F20" s="52"/>
       <c r="G20" s="30"/>
@@ -1928,11 +1990,11 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B22" s="27"/>
       <c r="C22" s="44" t="e">
-        <f>$I$1&amp;"."&amp;h0no&amp;"."&amp;h1no&amp;"."&amp;h2no</f>
+        <f>$I$1&amp;"."&amp;h0no&amp;"."&amp;h1no</f>
         <v>#NAME?</v>
       </c>
       <c r="D22" s="28"/>
@@ -1949,10 +2011,10 @@
       <c r="L22" s="1"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="17"/>
+      <c r="A23" s="6"/>
       <c r="B23" s="56"/>
-      <c r="C23" s="107"/>
-      <c r="D23" s="28"/>
+      <c r="C23" s="102"/>
+      <c r="D23" s="42"/>
       <c r="E23" s="103"/>
       <c r="F23" s="104"/>
       <c r="G23" s="105"/>
@@ -1964,7 +2026,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
-        <v>146</v>
+        <v>111</v>
       </c>
       <c r="B24" s="27"/>
       <c r="C24" s="44" t="e">
@@ -1999,278 +2061,319 @@
       <c r="L25" s="1"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="F26" s="51"/>
+      <c r="A26" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="B26" s="27"/>
+      <c r="C26" s="44" t="e">
+        <f>$I$1&amp;"."&amp;h0no&amp;"."&amp;h1no&amp;"."&amp;h2no</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D26" s="28"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="52"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="48"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="29">
+        <f>IF(ISNUMBER(F26),J26*F26,IF(ISNUMBER(H26),H26,J26))</f>
+        <v>0</v>
+      </c>
+      <c r="L26" s="1"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27" s="11"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="61"/>
-      <c r="I27" s="16"/>
-      <c r="L27" s="16"/>
+      <c r="A27" s="17"/>
+      <c r="B27" s="56"/>
+      <c r="C27" s="107"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="103"/>
+      <c r="F27" s="104"/>
+      <c r="G27" s="105"/>
+      <c r="H27" s="105"/>
+      <c r="I27" s="48"/>
+      <c r="J27" s="106"/>
+      <c r="K27" s="105"/>
+      <c r="L27" s="1"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B28" s="56"/>
-      <c r="C28" s="57"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="58"/>
-      <c r="F28" s="56"/>
-      <c r="G28" s="59" t="s">
-        <v>10</v>
-      </c>
-      <c r="H28" s="99" t="s">
-        <v>8</v>
-      </c>
-      <c r="I28" s="16"/>
-      <c r="K28" s="112">
-        <f>SUBTOTAL(9,K$5:K27)</f>
-        <v>0</v>
-      </c>
-      <c r="L28" s="16"/>
+      <c r="F28" s="51"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="56"/>
-      <c r="C29" s="57"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="58"/>
-      <c r="F29" s="56"/>
-      <c r="G29" s="59"/>
-      <c r="H29" s="63"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="61"/>
       <c r="I29" s="16"/>
-      <c r="K29" s="113"/>
       <c r="L29" s="16"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="60"/>
+      <c r="B30" s="56"/>
       <c r="C30" s="57"/>
       <c r="D30" s="28"/>
       <c r="E30" s="58"/>
       <c r="F30" s="56"/>
-      <c r="G30" s="59"/>
-      <c r="H30" s="62"/>
+      <c r="G30" s="59" t="s">
+        <v>10</v>
+      </c>
+      <c r="H30" s="99" t="s">
+        <v>8</v>
+      </c>
       <c r="I30" s="16"/>
-      <c r="K30" s="113"/>
+      <c r="K30" s="112">
+        <f>SUBTOTAL(9,K$7:K29)</f>
+        <v>0</v>
+      </c>
       <c r="L30" s="16"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="60"/>
+      <c r="B31" s="56"/>
       <c r="C31" s="57"/>
       <c r="D31" s="28"/>
       <c r="E31" s="58"/>
       <c r="F31" s="56"/>
-      <c r="G31" s="59" t="s">
-        <v>11</v>
-      </c>
-      <c r="H31" s="99" t="s">
-        <v>8</v>
-      </c>
+      <c r="G31" s="59"/>
+      <c r="H31" s="63"/>
       <c r="I31" s="16"/>
-      <c r="K31" s="112">
-        <f>SUBTOTAL(9,K$5:K27)</f>
-        <v>0</v>
-      </c>
+      <c r="K31" s="113"/>
       <c r="L31" s="16"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="43"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="63"/>
+      <c r="B32" s="60"/>
+      <c r="C32" s="57"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="58"/>
+      <c r="F32" s="56"/>
+      <c r="G32" s="59"/>
+      <c r="H32" s="62"/>
       <c r="I32" s="16"/>
+      <c r="K32" s="113"/>
       <c r="L32" s="16"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="55"/>
-      <c r="H35" s="86"/>
-      <c r="I35" s="1"/>
-      <c r="L35" s="1"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B36" s="81"/>
-      <c r="C36" s="82"/>
-      <c r="D36" s="81"/>
-      <c r="E36" s="83"/>
-      <c r="F36" s="84"/>
-      <c r="G36" s="85" t="s">
-        <v>7</v>
-      </c>
-      <c r="H36" s="88" t="s">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A33" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" s="60"/>
+      <c r="C33" s="57"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="58"/>
+      <c r="F33" s="56"/>
+      <c r="G33" s="59" t="s">
+        <v>11</v>
+      </c>
+      <c r="H33" s="99" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="1"/>
-      <c r="K36" s="112">
-        <f>SUBTOTAL(9,K$5:K35)</f>
+      <c r="I33" s="16"/>
+      <c r="K33" s="112">
+        <f>SUBTOTAL(9,K$7:K29)</f>
         <v>0</v>
       </c>
-      <c r="L36" s="1"/>
-    </row>
-    <row r="37" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L33" s="16"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A34" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="43"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="63"/>
+      <c r="I34" s="16"/>
+      <c r="L34" s="16"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="81"/>
-      <c r="C37" s="82"/>
-      <c r="D37" s="81"/>
-      <c r="E37" s="83"/>
-      <c r="F37" s="84"/>
-      <c r="G37" s="85"/>
-      <c r="H37" s="87"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="55"/>
+      <c r="H37" s="86"/>
       <c r="I37" s="1"/>
       <c r="L37" s="1"/>
     </row>
-    <row r="38" spans="1:12" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A39" s="17"/>
-      <c r="B39" s="27"/>
-      <c r="C39" s="44"/>
-      <c r="D39" s="28"/>
-      <c r="E39" s="41"/>
-      <c r="F39" s="52"/>
-      <c r="G39" s="30"/>
-      <c r="H39" s="31"/>
-      <c r="I39" s="48"/>
-      <c r="J39" s="32"/>
-      <c r="K39" s="29"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A42" s="101" t="s">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A38" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" s="81"/>
+      <c r="C38" s="82"/>
+      <c r="D38" s="81"/>
+      <c r="E38" s="83"/>
+      <c r="F38" s="84"/>
+      <c r="G38" s="85" t="s">
+        <v>7</v>
+      </c>
+      <c r="H38" s="88" t="s">
+        <v>8</v>
+      </c>
+      <c r="I38" s="1"/>
+      <c r="K38" s="112">
+        <f>SUBTOTAL(9,K$7:K37)</f>
+        <v>0</v>
+      </c>
+      <c r="L38" s="1"/>
+    </row>
+    <row r="39" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="81"/>
+      <c r="C39" s="82"/>
+      <c r="D39" s="81"/>
+      <c r="E39" s="83"/>
+      <c r="F39" s="84"/>
+      <c r="G39" s="85"/>
+      <c r="H39" s="87"/>
+      <c r="I39" s="1"/>
+      <c r="L39" s="1"/>
+    </row>
+    <row r="40" spans="1:12" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A41" s="17"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="44"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="41"/>
+      <c r="F41" s="52"/>
+      <c r="G41" s="30"/>
+      <c r="H41" s="31"/>
+      <c r="I41" s="48"/>
+      <c r="J41" s="32"/>
+      <c r="K41" s="29"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A44" s="101" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>154</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A45" s="110" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A46" s="110" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="110" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A48" s="111" t="s">
-        <v>145</v>
+      <c r="A48" s="110" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="110" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="111" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="110" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="110" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" s="110" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>116</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" s="111" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" s="111" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" s="111" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" s="111" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" s="111" t="s">
         <v>144</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" s="46" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" s="46" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" s="46" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" s="46" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" s="46" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" s="46" t="s">
         <v>148</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59" s="111" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" s="111" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" s="111" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" s="111" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" s="111" t="s">
         <v>150</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" s="46" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E9 E17 E26:E34" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E11 E19 E28:E36" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"-,No,m,m²,m³,%,Prov Sum,Lump Sum,Sum, Litre, hour, day"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2283,10 +2386,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2301,62 +2404,85 @@
       </c>
       <c r="B1" s="46"/>
     </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="121"/>
-      <c r="B3" s="121"/>
-      <c r="C3" s="122" t="str">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="46"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="46"/>
+      <c r="B3" s="124" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" s="124" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3" s="124" t="s">
+        <v>168</v>
+      </c>
+      <c r="E3" s="124" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="121"/>
+      <c r="B5" s="121"/>
+      <c r="C5" s="122" t="str">
         <f>BillTemplate!$B$1&amp;" "&amp;BillTemplate!$C$1</f>
         <v>Bill A: Test</v>
       </c>
-      <c r="D3" s="123" t="s">
+      <c r="D5" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="123">
+      <c r="E5" s="123">
         <f>BillTemplate!$K$1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="101" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="101" t="s">
         <v>100</v>
       </c>
-      <c r="B7" s="101"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="46" t="s">
-        <v>112</v>
-      </c>
-      <c r="B8" s="46"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="46" t="s">
-        <v>101</v>
-      </c>
-      <c r="B9" s="46"/>
+      <c r="B9" s="101"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="46" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="B10" s="46"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="101" t="s">
-        <v>155</v>
+      <c r="A11" s="46" t="s">
+        <v>101</v>
       </c>
       <c r="B11" s="46"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" s="46"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="101" t="s">
+        <v>155</v>
+      </c>
+      <c r="B13" s="46"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="B12" s="46"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="46" t="s">
+      <c r="B14" s="46"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="46" t="s">
         <v>103</v>
       </c>
-      <c r="B13" s="46"/>
+      <c r="B15" s="46"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="46" t="s">
+        <v>170</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>